<commit_message>
Updated list of canvassers
</commit_message>
<xml_diff>
--- a/Canvassers.xlsx
+++ b/Canvassers.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rba-col-dc01\RedirectedFolders\CCrowe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rba-col-dc01\RedirectedFolders\CCrowe\Desktop\areatracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553E8840-577E-4FE3-8C86-F73262CE2C7D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB659E2-286D-41C3-91D4-90A224440E51}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8685" xr2:uid="{D597821E-E3B5-453B-91CF-9FFAFF40941B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Vans" sheetId="1" r:id="rId1"/>
+    <sheet name="Permits" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>Employee</t>
   </si>
@@ -102,9 +103,6 @@
     <t>Cam Crowe</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>OFF</t>
   </si>
   <si>
@@ -123,9 +121,6 @@
     <t>Justin Blair</t>
   </si>
   <si>
-    <t>Canvassers</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
@@ -136,6 +131,60 @@
   </si>
   <si>
     <t>Van 2</t>
+  </si>
+  <si>
+    <t>Canvasser</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Broomfield</t>
+  </si>
+  <si>
+    <t>Permits have expiration dates</t>
+  </si>
+  <si>
+    <t>Expiration date</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Milliken</t>
+  </si>
+  <si>
+    <t>Johnstown</t>
+  </si>
+  <si>
+    <t>Greeley</t>
+  </si>
+  <si>
+    <t>Fort Collins</t>
+  </si>
+  <si>
+    <t>Plattesville</t>
+  </si>
+  <si>
+    <t>Frederick</t>
+  </si>
+  <si>
+    <t>Meade</t>
+  </si>
+  <si>
+    <t>Castle Rock</t>
+  </si>
+  <si>
+    <t>Lone Tree</t>
+  </si>
+  <si>
+    <t>Van A Hours</t>
+  </si>
+  <si>
+    <t>Van B Hours</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
@@ -528,564 +577,831 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA0B2BD-B0EF-4271-88A5-884C2310780B}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A2:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2">
         <v>8</v>
       </c>
-      <c r="F1">
+      <c r="G2">
         <v>7</v>
       </c>
-      <c r="G1">
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="I2">
         <v>6</v>
       </c>
-      <c r="I1">
+      <c r="J2">
         <v>6</v>
       </c>
-      <c r="J1">
+      <c r="K2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I4" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <f>IF(B5=1,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" t="s">
-        <v>27</v>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:C34" si="0">IF(B6=1,0,1)</f>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="2"/>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="D12" t="s">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>26</v>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="K15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>26</v>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="D17" t="s">
+      <c r="C17" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="2"/>
+      <c r="C19" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2"/>
+      <c r="C20" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2"/>
+      <c r="C21" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="2"/>
+      <c r="C22" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="D23" t="s">
+      <c r="C23" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="I24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="2"/>
+      <c r="C25" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E26" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E27" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E28" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E29" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E30" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="1" t="s">
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <f>SUM(B5:B33)</f>
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <f>SUM(C5:C34)</f>
+        <v>26</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="3">
+        <f>COUNTA($E5:$E33)</f>
+        <v>22</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" ref="F35:K35" si="1">$E35 - COUNTIF(F5:F33, "OFF")</f>
+        <v>17</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:K36" si="2">F35*F2</f>
+        <v>136</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="L36" s="4">
+        <f>SUM(F36:K36)</f>
+        <v>633</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <f>$B35*F2</f>
         <v>32</v>
       </c>
-      <c r="D34" s="3">
-        <f>COUNTA($D4:$D32)</f>
+      <c r="G37">
+        <f>$B35*G2</f>
+        <v>28</v>
+      </c>
+      <c r="H37">
+        <f>$B35*H2</f>
+        <v>24</v>
+      </c>
+      <c r="I37">
+        <f>$B35*I2</f>
+        <v>24</v>
+      </c>
+      <c r="J37">
+        <f>$B35*J2</f>
+        <v>24</v>
+      </c>
+      <c r="K37">
+        <f>$B35*K2</f>
         <v>22</v>
       </c>
-      <c r="E34" s="3">
-        <f t="shared" ref="E34:J34" si="0">$D34 - COUNTIF(E4:E32, "OFF")</f>
-        <v>17</v>
-      </c>
-      <c r="F34" s="3">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="G34" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="I34" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="J34" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35">
-        <f t="shared" ref="E35:J35" si="1">E34*E1</f>
-        <v>136</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
-        <v>133</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="1"/>
+      <c r="L37" s="4">
+        <f t="shared" ref="L37:L38" si="3">SUM(F37:K37)</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38">
+        <f>$B35*F2</f>
+        <v>32</v>
+      </c>
+      <c r="G38">
+        <f>$B35*G2</f>
+        <v>28</v>
+      </c>
+      <c r="H38">
+        <f>$B35*H2</f>
+        <v>24</v>
+      </c>
+      <c r="I38">
+        <f>$B35*I2</f>
+        <v>24</v>
+      </c>
+      <c r="J38">
+        <f>$B35*J2</f>
+        <v>24</v>
+      </c>
+      <c r="K38">
+        <f>$B35*K2</f>
         <v>22</v>
       </c>
-      <c r="K35" s="4">
-        <f>SUM(E35:J35)</f>
-        <v>663</v>
+      <c r="L38" s="4">
+        <f t="shared" si="3"/>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D7:J25">
-    <sortCondition ref="D7:D25"/>
+  <sortState ref="E8:K26">
+    <sortCondition ref="E8:E26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E717928-7A80-47CB-B92F-15428AD7721B}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated canvass worksheet SR
</commit_message>
<xml_diff>
--- a/Canvassers.xlsx
+++ b/Canvassers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rba-col-dc01\RedirectedFolders\CCrowe\Desktop\areatracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC9A6EB-2237-45DC-91BA-854D35A51109}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B967C27-C330-443B-87F6-4419E2B9E06B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8685" activeTab="1" xr2:uid="{D597821E-E3B5-453B-91CF-9FFAFF40941B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8685" xr2:uid="{D597821E-E3B5-453B-91CF-9FFAFF40941B}"/>
   </bookViews>
   <sheets>
     <sheet name="Vans" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Employee</t>
   </si>
@@ -76,12 +76,6 @@
     <t>Dom Rael</t>
   </si>
   <si>
-    <t>Breanna Ybarra</t>
-  </si>
-  <si>
-    <t>Doncey Albin</t>
-  </si>
-  <si>
     <t>Bill Canfield</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Tim Raleigh</t>
   </si>
   <si>
-    <t>Justin Blair</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
@@ -185,6 +176,12 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -252,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -263,6 +260,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,32 +575,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA0B2BD-B0EF-4271-88A5-884C2310780B}">
-  <dimension ref="A2:L38"/>
+  <dimension ref="A2:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>7</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
       </c>
       <c r="I2">
         <v>6</v>
@@ -611,60 +606,69 @@
         <v>6</v>
       </c>
       <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
       <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="5">
         <f>IF(B5=1,0,1)</f>
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
+      <c r="D5" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -672,95 +676,100 @@
         <f t="shared" ref="C6:C34" si="0">IF(B6=1,0,1)</f>
         <v>0</v>
       </c>
-      <c r="D6" t="s">
-        <v>26</v>
+      <c r="D6" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
+      <c r="D7" s="6"/>
       <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" s="6"/>
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2"/>
+      <c r="D9" s="6"/>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2"/>
+      <c r="D10" s="6"/>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>1</v>
       </c>
@@ -768,19 +777,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="2"/>
+      <c r="D11" s="6"/>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>1</v>
       </c>
@@ -788,47 +798,41 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D12" s="6"/>
+      <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D13" s="6"/>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>1</v>
       </c>
@@ -836,499 +840,490 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>25</v>
+      <c r="D14" s="6"/>
+      <c r="F14" t="s">
+        <v>26</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="K14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D15" s="6"/>
+      <c r="F15" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E16" t="s">
+      <c r="D16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D17" s="6"/>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="2"/>
+      <c r="D18" s="6"/>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E19" t="s">
+      <c r="D19" s="6"/>
+      <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="D20" s="6"/>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E21" t="s">
+      <c r="D21" s="6"/>
+      <c r="F21" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="2"/>
+      <c r="D22" s="6"/>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D23" s="6"/>
+      <c r="F23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="2"/>
+      <c r="D25" s="6"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
       <c r="C26" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="D27" s="6"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="D28" s="6"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="D29" s="6"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="D30" s="6"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="D31" s="6"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="D32" s="6"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="D33" s="6"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="D34" s="6"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B35">
         <f>SUM(B5:B33)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C35">
         <f>SUM(C5:C34)</f>
-        <v>26</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="3">
-        <f>COUNTA($E5:$E33)</f>
-        <v>22</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="3">
-        <f t="shared" ref="F35:K35" si="1">$E35 - COUNTIF(F5:F33, "OFF")</f>
-        <v>17</v>
+        <f>COUNTA($F5:$F33)</f>
+        <v>19</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" ref="G35:L35" si="1">$F35 - COUNTIF(G5:G33, "OFF")</f>
+        <v>16</v>
       </c>
       <c r="H35" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I35" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J35" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K35" s="3">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36">
-        <f t="shared" ref="F36:K36" si="2">F35*F2</f>
-        <v>136</v>
+        <v>17</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>28</v>
       </c>
       <c r="G36">
-        <f t="shared" si="2"/>
-        <v>133</v>
+        <f t="shared" ref="G36:L36" si="2">G35*G2</f>
+        <v>128</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="I36">
         <f t="shared" si="2"/>
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J36">
         <f t="shared" si="2"/>
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="K36">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="L36" s="4">
-        <f>SUM(F36:K36)</f>
-        <v>633</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37">
-        <f>$B35*F2</f>
-        <v>32</v>
+        <v>102</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="M36" s="4">
+        <f>SUM(G36:L36)</f>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>47</v>
       </c>
       <c r="G37">
-        <f>$B35*G2</f>
-        <v>28</v>
+        <f t="shared" ref="G37:L37" si="3">$B35*G2</f>
+        <v>40</v>
       </c>
       <c r="H37">
-        <f>$B35*H2</f>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>35</v>
       </c>
       <c r="I37">
-        <f>$B35*I2</f>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>30</v>
       </c>
       <c r="J37">
-        <f>$B35*J2</f>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>30</v>
       </c>
       <c r="K37">
-        <f>$B35*K2</f>
-        <v>22</v>
-      </c>
-      <c r="L37" s="4">
-        <f t="shared" ref="L37:L38" si="3">SUM(F37:K37)</f>
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F38">
-        <f>$C35*F2</f>
-        <v>208</v>
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="3"/>
+        <v>27.5</v>
+      </c>
+      <c r="M37" s="4">
+        <f t="shared" ref="M37:M38" si="4">SUM(G37:L37)</f>
+        <v>192.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>48</v>
       </c>
       <c r="G38">
-        <f>$C35*G2</f>
-        <v>182</v>
+        <f t="shared" ref="G38:L38" si="5">$C35*G2</f>
+        <v>200</v>
       </c>
       <c r="H38">
-        <f>$C35*H2</f>
-        <v>156</v>
+        <f t="shared" si="5"/>
+        <v>175</v>
       </c>
       <c r="I38">
-        <f>$C35*I2</f>
-        <v>156</v>
+        <f t="shared" si="5"/>
+        <v>150</v>
       </c>
       <c r="J38">
-        <f>$C35*J2</f>
-        <v>156</v>
+        <f t="shared" si="5"/>
+        <v>150</v>
       </c>
       <c r="K38">
-        <f>$C35*K2</f>
-        <v>143</v>
-      </c>
-      <c r="L38" s="4">
-        <f t="shared" si="3"/>
-        <v>1001</v>
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="5"/>
+        <v>137.5</v>
+      </c>
+      <c r="M38" s="4">
+        <f t="shared" si="4"/>
+        <v>962.5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="E8:K26">
-    <sortCondition ref="E8:E26"/>
+  <sortState ref="F8:L26">
+    <sortCondition ref="F8:F26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1339,7 +1334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E717928-7A80-47CB-B92F-15428AD7721B}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1351,272 +1346,272 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" t="str">
-        <f>B2</f>
+        <f t="shared" ref="B5:L5" si="0">B2</f>
         <v>Parker</v>
       </c>
       <c r="C5" t="str">
-        <f>C2</f>
+        <f t="shared" si="0"/>
         <v>Broomfield</v>
       </c>
       <c r="D5" t="str">
-        <f>D2</f>
+        <f t="shared" si="0"/>
         <v>Milliken</v>
       </c>
       <c r="E5" t="str">
-        <f>E2</f>
+        <f t="shared" si="0"/>
         <v>Johnstown</v>
       </c>
       <c r="F5" t="str">
-        <f>F2</f>
+        <f t="shared" si="0"/>
         <v>Greeley</v>
       </c>
       <c r="G5" t="str">
-        <f>G2</f>
+        <f t="shared" si="0"/>
         <v>Fort Collins</v>
       </c>
       <c r="H5" t="str">
-        <f>H2</f>
+        <f t="shared" si="0"/>
         <v>Plattesville</v>
       </c>
       <c r="I5" t="str">
-        <f>I2</f>
+        <f t="shared" si="0"/>
         <v>Frederick</v>
       </c>
       <c r="J5" t="str">
-        <f>J2</f>
+        <f t="shared" si="0"/>
         <v>Meade</v>
       </c>
       <c r="K5" t="str">
-        <f>K2</f>
+        <f t="shared" si="0"/>
         <v>Castle Rock</v>
       </c>
       <c r="L5" t="str">
-        <f>L2</f>
+        <f t="shared" si="0"/>
         <v>Lone Tree</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>Vans!E5</f>
+        <f>Vans!F5</f>
         <v>Spencer Russell</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>Vans!E6</f>
+        <f>Vans!F6</f>
         <v>Adam Belvin</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>Vans!E7</f>
+        <f>Vans!F7</f>
         <v>Cam Crowe</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>Vans!E8</f>
+        <f>Vans!F8</f>
         <v>Allan Woodall</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>Vans!E9</f>
+        <f>Vans!F9</f>
         <v>Bill Canfield</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>Vans!E10</f>
-        <v>Breanna Ybarra</v>
+      <c r="A11" t="e">
+        <f>Vans!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>Vans!E11</f>
+        <f>Vans!F11</f>
         <v>Colton Sasa</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>Vans!E12</f>
+        <f>Vans!F12</f>
         <v>Dom Rael</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f>Vans!E13</f>
-        <v>Doncey Albin</v>
+      <c r="A14" t="e">
+        <f>Vans!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>Vans!E14</f>
+        <f>Vans!F14</f>
         <v>Frank Harritt</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>Vans!E15</f>
+        <f>Vans!F15</f>
         <v>Garrett Cumpster</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>Vans!E16</f>
+        <f>Vans!F16</f>
         <v>Jared Shelden</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f>Vans!E17</f>
-        <v>Justin Blair</v>
+      <c r="A18" t="e">
+        <f>Vans!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>Vans!E18</f>
+        <f>Vans!F18</f>
         <v>Lucas Reilly</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>Vans!E19</f>
+        <f>Vans!F19</f>
         <v>Michael Finke</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>Vans!E20</f>
+        <f>Vans!F20</f>
         <v>Nick Visscher</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>Vans!E21</f>
+        <f>Vans!F21</f>
         <v>Pressley Farrell</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>Vans!E22</f>
+        <f>Vans!F22</f>
         <v>Rob Paddock</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>Vans!E23</f>
+        <f>Vans!F23</f>
         <v>Ryan McComber</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>Vans!E24</f>
+        <f>Vans!F17</f>
         <v>Sam Sammarco</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>Vans!E25</f>
+        <f>Vans!F10</f>
         <v>Stephen Vaulton</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>Vans!E26</f>
+        <f>Vans!F13</f>
         <v>Tim Raleigh</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>Vans!E27</f>
+        <f>Vans!F27</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>Vans!E28</f>
+        <f>Vans!F28</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>Vans!E29</f>
+        <f>Vans!F29</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>Vans!E30</f>
+        <f>Vans!F30</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>Vans!E31</f>
+        <f>Vans!F31</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>Vans!E32</f>
+        <f>Vans!F32</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>Vans!E33</f>
+        <f>Vans!F33</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>